<commit_message>
Fixing common field name error
</commit_message>
<xml_diff>
--- a/configuration/fields.xlsx
+++ b/configuration/fields.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tauex-my.sharepoint.com/personal/kerenha_tauex_tau_ac_il/Documents/Documents/ArcGIS/pty_framework/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="406" documentId="13_ncr:1_{42DDB87E-81E9-4226-9973-413C4AA9401D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AACF957F-1E98-4110-9300-114AECC63841}"/>
+  <xr:revisionPtr revIDLastSave="445" documentId="13_ncr:1_{42DDB87E-81E9-4226-9973-413C4AA9401D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04B49F21-9103-48AE-998F-E6100F907CD6}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="673" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="673" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3391" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3088" uniqueCount="514">
   <si>
     <t>OBJECTID</t>
   </si>
@@ -1582,30 +1582,6 @@
     <t>"אין"</t>
   </si>
   <si>
-    <t>points_discussion_2</t>
-  </si>
-  <si>
-    <t>הרכב מינים_ארכיון</t>
-  </si>
-  <si>
-    <t>% עצים מתים</t>
-  </si>
-  <si>
-    <t>% עצים נטויים</t>
-  </si>
-  <si>
-    <t>% עצים שבורים</t>
-  </si>
-  <si>
-    <t>% עצים שרופים</t>
-  </si>
-  <si>
-    <t>order</t>
-  </si>
-  <si>
-    <t>visible</t>
-  </si>
-  <si>
     <t>NoteNumber</t>
   </si>
   <si>
@@ -1619,6 +1595,15 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>common_error</t>
+  </si>
+  <si>
+    <t>ForestName</t>
+  </si>
+  <si>
+    <t>AgeCategory</t>
   </si>
 </sst>
 </file>
@@ -1972,7 +1957,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -2259,7 +2244,8 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10029,10 +10015,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B81B3B6-A5EA-43DC-9DF2-5745324BB6CB}">
-  <dimension ref="A1:L154"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="B24" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -10045,9 +10031,10 @@
     <col min="6" max="6" width="14.90625" customWidth="1"/>
     <col min="7" max="7" width="6.36328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.54296875" customWidth="1"/>
+    <col min="11" max="11" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="96" t="s">
         <v>1</v>
       </c>
@@ -10078,14 +10065,11 @@
       <c r="J1" s="111" t="s">
         <v>502</v>
       </c>
-      <c r="K1" s="111" t="s">
-        <v>512</v>
-      </c>
-      <c r="L1" s="111" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K1" s="113" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="98">
         <v>30000</v>
       </c>
@@ -10105,7 +10089,7 @@
       <c r="G2" s="101"/>
       <c r="H2" s="102"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="98">
         <v>30001</v>
       </c>
@@ -10125,7 +10109,7 @@
       <c r="G3" s="105"/>
       <c r="H3" s="106"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="98">
         <v>30002</v>
       </c>
@@ -10145,7 +10129,7 @@
       <c r="G4" s="101"/>
       <c r="H4" s="102"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="98">
         <v>30003</v>
       </c>
@@ -10167,7 +10151,7 @@
       <c r="G5" s="105"/>
       <c r="H5" s="106"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="98">
         <v>30004</v>
       </c>
@@ -10187,7 +10171,7 @@
       <c r="G6" s="101"/>
       <c r="H6" s="102"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="98">
         <v>30005</v>
       </c>
@@ -10209,7 +10193,7 @@
       <c r="G7" s="105"/>
       <c r="H7" s="106"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="98">
         <v>30006</v>
       </c>
@@ -10229,7 +10213,7 @@
       <c r="G8" s="101"/>
       <c r="H8" s="102"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="98">
         <v>30007</v>
       </c>
@@ -10252,7 +10236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="98">
         <v>30008</v>
       </c>
@@ -10275,7 +10259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="98">
         <v>30009</v>
       </c>
@@ -10298,7 +10282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="98">
         <v>30010</v>
       </c>
@@ -10321,7 +10305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="98">
         <v>30011</v>
       </c>
@@ -10344,7 +10328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="98">
         <v>30012</v>
       </c>
@@ -10367,7 +10351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="98">
         <v>30013</v>
       </c>
@@ -10390,7 +10374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="98">
         <v>30014</v>
       </c>
@@ -10413,7 +10397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="98">
         <v>30015</v>
       </c>
@@ -10436,7 +10420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="98">
         <v>30016</v>
       </c>
@@ -10459,7 +10443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="98">
         <v>30017</v>
       </c>
@@ -10482,7 +10466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="98">
         <v>30018</v>
       </c>
@@ -10505,7 +10489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="98">
         <v>30019</v>
       </c>
@@ -10528,7 +10512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="98">
         <v>30020</v>
       </c>
@@ -10553,7 +10537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="98">
         <v>30021</v>
       </c>
@@ -10576,7 +10560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="98">
         <v>30022</v>
       </c>
@@ -10599,7 +10583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="98">
         <v>30023</v>
       </c>
@@ -10622,7 +10606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="98">
         <v>30024</v>
       </c>
@@ -10645,7 +10629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="98">
         <v>30025</v>
       </c>
@@ -10670,7 +10654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="98">
         <v>30026</v>
       </c>
@@ -10693,7 +10677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="98">
         <v>30027</v>
       </c>
@@ -10716,7 +10700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="98">
         <v>30028</v>
       </c>
@@ -10724,7 +10708,7 @@
         <v>464</v>
       </c>
       <c r="C30" s="107" t="s">
-        <v>449</v>
+        <v>17</v>
       </c>
       <c r="D30" s="100" t="s">
         <v>450</v>
@@ -10738,8 +10722,11 @@
       <c r="J30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30" s="112" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="98">
         <v>30029</v>
       </c>
@@ -10762,99 +10749,103 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="98">
-        <v>30030</v>
-      </c>
-      <c r="B32" s="100" t="s">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="98"/>
+      <c r="B32" s="104" t="s">
         <v>464</v>
       </c>
-      <c r="C32" s="107" t="s">
-        <v>23</v>
-      </c>
-      <c r="D32" s="107" t="s">
-        <v>24</v>
-      </c>
-      <c r="E32" s="107" t="s">
-        <v>444</v>
-      </c>
-      <c r="F32" s="100"/>
-      <c r="G32" s="101"/>
-      <c r="H32" s="102"/>
+      <c r="C32" s="103" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="103" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="103" t="s">
+        <v>429</v>
+      </c>
+      <c r="F32" s="104"/>
+      <c r="G32" s="105"/>
+      <c r="H32" s="106"/>
       <c r="J32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32" s="112" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="98">
-        <v>30031</v>
-      </c>
-      <c r="B33" s="104" t="s">
+        <v>30030</v>
+      </c>
+      <c r="B33" s="100" t="s">
         <v>464</v>
       </c>
-      <c r="C33" s="103" t="s">
-        <v>25</v>
-      </c>
-      <c r="D33" s="103" t="s">
-        <v>26</v>
-      </c>
-      <c r="E33" s="103" t="s">
+      <c r="C33" s="107" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" s="107" t="s">
+        <v>24</v>
+      </c>
+      <c r="E33" s="107" t="s">
         <v>444</v>
       </c>
-      <c r="F33" s="104"/>
-      <c r="G33" s="105"/>
-      <c r="H33" s="106"/>
+      <c r="F33" s="100"/>
+      <c r="G33" s="101"/>
+      <c r="H33" s="102"/>
       <c r="J33">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="98">
-        <v>30032</v>
-      </c>
-      <c r="B34" s="100" t="s">
+        <v>30031</v>
+      </c>
+      <c r="B34" s="104" t="s">
         <v>464</v>
       </c>
-      <c r="C34" s="107" t="s">
-        <v>446</v>
-      </c>
-      <c r="D34" s="100" t="s">
-        <v>448</v>
-      </c>
-      <c r="E34" s="107" t="s">
+      <c r="C34" s="103" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="103" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="103" t="s">
         <v>444</v>
       </c>
-      <c r="F34" s="100"/>
-      <c r="G34" s="101"/>
-      <c r="H34" s="102"/>
+      <c r="F34" s="104"/>
+      <c r="G34" s="105"/>
+      <c r="H34" s="106"/>
       <c r="J34">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="98">
-        <v>30033</v>
-      </c>
-      <c r="B35" s="104" t="s">
+        <v>30032</v>
+      </c>
+      <c r="B35" s="100" t="s">
         <v>464</v>
       </c>
-      <c r="C35" s="103" t="s">
-        <v>447</v>
-      </c>
-      <c r="D35" s="104" t="s">
+      <c r="C35" s="107" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="100" t="s">
         <v>448</v>
       </c>
-      <c r="E35" s="104" t="s">
-        <v>429</v>
-      </c>
-      <c r="F35" s="104"/>
-      <c r="G35" s="105"/>
-      <c r="H35" s="106"/>
+      <c r="E35" s="107" t="s">
+        <v>444</v>
+      </c>
+      <c r="F35" s="100"/>
+      <c r="G35" s="101"/>
+      <c r="H35" s="102"/>
       <c r="J35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K35" s="112" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="98">
         <v>30034</v>
       </c>
@@ -10877,7 +10868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="98">
         <v>30035</v>
       </c>
@@ -10899,8 +10890,11 @@
       <c r="J37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K37" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="98">
         <v>30036</v>
       </c>
@@ -10925,7 +10919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="98">
         <v>30037</v>
       </c>
@@ -10950,7 +10944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="98">
         <v>30038</v>
       </c>
@@ -10975,7 +10969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="98">
         <v>30039</v>
       </c>
@@ -11000,7 +10994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="98">
         <v>30040</v>
       </c>
@@ -11025,7 +11019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="98">
         <v>30041</v>
       </c>
@@ -11050,7 +11044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="98">
         <v>30042</v>
       </c>
@@ -11075,7 +11069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="98">
         <v>30043</v>
       </c>
@@ -11098,7 +11092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="98">
         <v>30044</v>
       </c>
@@ -11106,7 +11100,7 @@
         <v>483</v>
       </c>
       <c r="C46" s="107" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="D46" s="100" t="s">
         <v>437</v>
@@ -11118,7 +11112,7 @@
       <c r="G46" s="101"/>
       <c r="H46" s="100"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="98">
         <v>30045</v>
       </c>
@@ -11129,7 +11123,7 @@
         <v>485</v>
       </c>
       <c r="D47" s="104" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="E47" s="104" t="s">
         <v>429</v>
@@ -11138,7 +11132,7 @@
       <c r="G47" s="105"/>
       <c r="H47" s="104"/>
     </row>
-    <row r="48" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A48" s="98">
         <v>30046</v>
       </c>
@@ -11149,7 +11143,7 @@
         <v>486</v>
       </c>
       <c r="D48" s="109" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="E48" s="104" t="s">
         <v>429</v>
@@ -11158,7 +11152,7 @@
       <c r="G48" s="101"/>
       <c r="H48" s="100"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="98">
         <v>30047</v>
       </c>
@@ -11180,7 +11174,7 @@
       <c r="G49" s="105"/>
       <c r="H49" s="104"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="98">
         <v>30048</v>
       </c>
@@ -11200,7 +11194,7 @@
       <c r="G50" s="101"/>
       <c r="H50" s="102"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="98">
         <v>30049</v>
       </c>
@@ -11208,21 +11202,21 @@
         <v>483</v>
       </c>
       <c r="C51" s="103" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="D51" s="104" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="E51" s="104" t="s">
         <v>429</v>
       </c>
       <c r="F51" s="104" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="G51" s="105"/>
       <c r="H51" s="106"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="98">
         <v>30050</v>
       </c>
@@ -11243,1587 +11237,6 @@
       </c>
       <c r="G52" s="101"/>
       <c r="H52" s="102"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B53" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C53" t="s">
-        <v>12</v>
-      </c>
-      <c r="D53" t="s">
-        <v>13</v>
-      </c>
-      <c r="K53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B54" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C54" t="s">
-        <v>17</v>
-      </c>
-      <c r="D54" t="s">
-        <v>18</v>
-      </c>
-      <c r="K54">
-        <v>2</v>
-      </c>
-      <c r="L54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B55" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C55" t="s">
-        <v>21</v>
-      </c>
-      <c r="D55" t="s">
-        <v>22</v>
-      </c>
-      <c r="K55">
-        <v>3</v>
-      </c>
-      <c r="L55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B56" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C56" t="s">
-        <v>19</v>
-      </c>
-      <c r="D56" t="s">
-        <v>20</v>
-      </c>
-      <c r="K56">
-        <v>4</v>
-      </c>
-      <c r="L56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B57" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C57" t="s">
-        <v>23</v>
-      </c>
-      <c r="D57" t="s">
-        <v>24</v>
-      </c>
-      <c r="K57">
-        <v>5</v>
-      </c>
-      <c r="L57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B58" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C58" t="s">
-        <v>25</v>
-      </c>
-      <c r="D58" t="s">
-        <v>26</v>
-      </c>
-      <c r="K58">
-        <v>6</v>
-      </c>
-      <c r="L58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B59" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C59" t="s">
-        <v>15</v>
-      </c>
-      <c r="D59" t="s">
-        <v>16</v>
-      </c>
-      <c r="K59">
-        <v>7</v>
-      </c>
-      <c r="L59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B60" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C60" t="s">
-        <v>27</v>
-      </c>
-      <c r="D60" t="s">
-        <v>28</v>
-      </c>
-      <c r="K60">
-        <v>8</v>
-      </c>
-      <c r="L60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B61" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C61" t="s">
-        <v>29</v>
-      </c>
-      <c r="D61" t="s">
-        <v>30</v>
-      </c>
-      <c r="K61">
-        <v>9</v>
-      </c>
-      <c r="L61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B62" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C62" t="s">
-        <v>31</v>
-      </c>
-      <c r="D62" t="s">
-        <v>32</v>
-      </c>
-      <c r="K62">
-        <v>10</v>
-      </c>
-      <c r="L62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B63" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C63" t="s">
-        <v>33</v>
-      </c>
-      <c r="D63" t="s">
-        <v>507</v>
-      </c>
-      <c r="K63">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B64" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C64" t="s">
-        <v>35</v>
-      </c>
-      <c r="D64" t="s">
-        <v>36</v>
-      </c>
-      <c r="K64">
-        <v>12</v>
-      </c>
-      <c r="L64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B65" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C65" t="s">
-        <v>37</v>
-      </c>
-      <c r="D65" t="s">
-        <v>38</v>
-      </c>
-      <c r="K65">
-        <v>13</v>
-      </c>
-      <c r="L65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B66" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C66" t="s">
-        <v>55</v>
-      </c>
-      <c r="D66" t="s">
-        <v>56</v>
-      </c>
-      <c r="K66">
-        <v>14</v>
-      </c>
-      <c r="L66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B67" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C67" t="s">
-        <v>39</v>
-      </c>
-      <c r="D67" t="s">
-        <v>40</v>
-      </c>
-      <c r="K67">
-        <v>15</v>
-      </c>
-      <c r="L67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B68" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C68" t="s">
-        <v>41</v>
-      </c>
-      <c r="D68" t="s">
-        <v>42</v>
-      </c>
-      <c r="K68">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B69" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C69" t="s">
-        <v>43</v>
-      </c>
-      <c r="D69" t="s">
-        <v>44</v>
-      </c>
-      <c r="K69">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="70" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B70" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C70" t="s">
-        <v>202</v>
-      </c>
-      <c r="D70" t="s">
-        <v>34</v>
-      </c>
-      <c r="K70">
-        <v>18</v>
-      </c>
-      <c r="L70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B71" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C71" t="s">
-        <v>200</v>
-      </c>
-      <c r="D71" t="s">
-        <v>201</v>
-      </c>
-      <c r="K71">
-        <v>19</v>
-      </c>
-      <c r="L71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B72" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C72" t="s">
-        <v>49</v>
-      </c>
-      <c r="D72" t="s">
-        <v>50</v>
-      </c>
-      <c r="K72">
-        <v>20</v>
-      </c>
-      <c r="L72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B73" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C73" t="s">
-        <v>52</v>
-      </c>
-      <c r="D73" t="s">
-        <v>53</v>
-      </c>
-      <c r="K73">
-        <v>21</v>
-      </c>
-      <c r="L73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B74" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C74" t="s">
-        <v>184</v>
-      </c>
-      <c r="D74" t="s">
-        <v>185</v>
-      </c>
-      <c r="K74">
-        <v>22</v>
-      </c>
-      <c r="L74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B75" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C75" t="s">
-        <v>186</v>
-      </c>
-      <c r="D75" t="s">
-        <v>187</v>
-      </c>
-      <c r="K75">
-        <v>23</v>
-      </c>
-      <c r="L75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B76" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C76" t="s">
-        <v>188</v>
-      </c>
-      <c r="D76" t="s">
-        <v>189</v>
-      </c>
-      <c r="K76">
-        <v>24</v>
-      </c>
-      <c r="L76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B77" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C77" t="s">
-        <v>190</v>
-      </c>
-      <c r="D77" t="s">
-        <v>191</v>
-      </c>
-      <c r="K77">
-        <v>25</v>
-      </c>
-      <c r="L77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B78" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C78" t="s">
-        <v>192</v>
-      </c>
-      <c r="D78" t="s">
-        <v>193</v>
-      </c>
-      <c r="K78">
-        <v>26</v>
-      </c>
-      <c r="L78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B79" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C79" t="s">
-        <v>194</v>
-      </c>
-      <c r="D79" t="s">
-        <v>195</v>
-      </c>
-      <c r="K79">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B80" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C80" t="s">
-        <v>196</v>
-      </c>
-      <c r="D80" t="s">
-        <v>197</v>
-      </c>
-      <c r="K80">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B81" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C81" t="s">
-        <v>198</v>
-      </c>
-      <c r="D81" t="s">
-        <v>199</v>
-      </c>
-      <c r="K81">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B82" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C82" t="s">
-        <v>173</v>
-      </c>
-      <c r="D82" t="s">
-        <v>174</v>
-      </c>
-      <c r="K82">
-        <v>30</v>
-      </c>
-      <c r="L82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B83" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C83" t="s">
-        <v>176</v>
-      </c>
-      <c r="D83" t="s">
-        <v>177</v>
-      </c>
-      <c r="K83">
-        <v>31</v>
-      </c>
-      <c r="L83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B84" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C84" t="s">
-        <v>58</v>
-      </c>
-      <c r="D84" t="s">
-        <v>59</v>
-      </c>
-      <c r="K84">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B85" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C85" t="s">
-        <v>60</v>
-      </c>
-      <c r="D85" t="s">
-        <v>61</v>
-      </c>
-      <c r="K85">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B86" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C86" t="s">
-        <v>62</v>
-      </c>
-      <c r="D86" t="s">
-        <v>63</v>
-      </c>
-      <c r="K86">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B87" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C87" t="s">
-        <v>65</v>
-      </c>
-      <c r="D87" t="s">
-        <v>66</v>
-      </c>
-      <c r="K87">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B88" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C88" t="s">
-        <v>67</v>
-      </c>
-      <c r="D88" t="s">
-        <v>67</v>
-      </c>
-      <c r="K88">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B89" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C89" t="s">
-        <v>68</v>
-      </c>
-      <c r="D89" t="s">
-        <v>68</v>
-      </c>
-      <c r="K89">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B90" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C90" t="s">
-        <v>69</v>
-      </c>
-      <c r="D90" t="s">
-        <v>69</v>
-      </c>
-      <c r="K90">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B91" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C91" t="s">
-        <v>70</v>
-      </c>
-      <c r="D91" t="s">
-        <v>70</v>
-      </c>
-      <c r="K91">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B92" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C92" t="s">
-        <v>71</v>
-      </c>
-      <c r="D92" t="s">
-        <v>71</v>
-      </c>
-      <c r="K92">
-        <v>40</v>
-      </c>
-      <c r="L92">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B93" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C93" t="s">
-        <v>72</v>
-      </c>
-      <c r="D93" t="s">
-        <v>72</v>
-      </c>
-      <c r="K93">
-        <v>41</v>
-      </c>
-      <c r="L93">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B94" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C94" t="s">
-        <v>73</v>
-      </c>
-      <c r="D94" t="s">
-        <v>73</v>
-      </c>
-      <c r="K94">
-        <v>42</v>
-      </c>
-      <c r="L94">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B95" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C95" t="s">
-        <v>74</v>
-      </c>
-      <c r="D95" t="s">
-        <v>75</v>
-      </c>
-      <c r="K95">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="96" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B96" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C96" t="s">
-        <v>76</v>
-      </c>
-      <c r="D96" t="s">
-        <v>77</v>
-      </c>
-      <c r="K96">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="97" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B97" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C97" t="s">
-        <v>79</v>
-      </c>
-      <c r="D97" t="s">
-        <v>80</v>
-      </c>
-      <c r="K97">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="98" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B98" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C98" t="s">
-        <v>81</v>
-      </c>
-      <c r="D98" t="s">
-        <v>81</v>
-      </c>
-      <c r="K98">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="99" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B99" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C99" t="s">
-        <v>82</v>
-      </c>
-      <c r="D99" t="s">
-        <v>82</v>
-      </c>
-      <c r="K99">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="100" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B100" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C100" t="s">
-        <v>83</v>
-      </c>
-      <c r="D100" t="s">
-        <v>83</v>
-      </c>
-      <c r="K100">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="101" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B101" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C101" t="s">
-        <v>84</v>
-      </c>
-      <c r="D101" t="s">
-        <v>84</v>
-      </c>
-      <c r="K101">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="102" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B102" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C102" t="s">
-        <v>85</v>
-      </c>
-      <c r="D102" t="s">
-        <v>85</v>
-      </c>
-      <c r="K102">
-        <v>50</v>
-      </c>
-      <c r="L102">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B103" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C103" t="s">
-        <v>86</v>
-      </c>
-      <c r="D103" t="s">
-        <v>86</v>
-      </c>
-      <c r="K103">
-        <v>51</v>
-      </c>
-      <c r="L103">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B104" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C104" t="s">
-        <v>87</v>
-      </c>
-      <c r="D104" t="s">
-        <v>87</v>
-      </c>
-      <c r="K104">
-        <v>52</v>
-      </c>
-      <c r="L104">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B105" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C105" t="s">
-        <v>88</v>
-      </c>
-      <c r="D105" t="s">
-        <v>89</v>
-      </c>
-      <c r="K105">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="106" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B106" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C106" t="s">
-        <v>90</v>
-      </c>
-      <c r="D106" t="s">
-        <v>91</v>
-      </c>
-      <c r="K106">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="107" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B107" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C107" t="s">
-        <v>93</v>
-      </c>
-      <c r="D107" t="s">
-        <v>94</v>
-      </c>
-      <c r="K107">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="108" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B108" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C108" t="s">
-        <v>95</v>
-      </c>
-      <c r="D108" t="s">
-        <v>95</v>
-      </c>
-      <c r="K108">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="109" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B109" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C109" t="s">
-        <v>96</v>
-      </c>
-      <c r="D109" t="s">
-        <v>96</v>
-      </c>
-      <c r="K109">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="110" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B110" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C110" t="s">
-        <v>97</v>
-      </c>
-      <c r="D110" t="s">
-        <v>97</v>
-      </c>
-      <c r="K110">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="111" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B111" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C111" t="s">
-        <v>98</v>
-      </c>
-      <c r="D111" t="s">
-        <v>98</v>
-      </c>
-      <c r="K111">
-        <v>59</v>
-      </c>
-      <c r="L111">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B112" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C112" t="s">
-        <v>99</v>
-      </c>
-      <c r="D112" t="s">
-        <v>99</v>
-      </c>
-      <c r="K112">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="113" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B113" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C113" t="s">
-        <v>100</v>
-      </c>
-      <c r="D113" t="s">
-        <v>100</v>
-      </c>
-      <c r="K113">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="114" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B114" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C114" t="s">
-        <v>101</v>
-      </c>
-      <c r="D114" t="s">
-        <v>101</v>
-      </c>
-      <c r="K114">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="115" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B115" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C115" t="s">
-        <v>102</v>
-      </c>
-      <c r="D115" t="s">
-        <v>103</v>
-      </c>
-      <c r="K115">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="116" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B116" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C116" t="s">
-        <v>180</v>
-      </c>
-      <c r="D116" t="s">
-        <v>181</v>
-      </c>
-      <c r="K116">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="117" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B117" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C117" t="s">
-        <v>182</v>
-      </c>
-      <c r="D117" t="s">
-        <v>183</v>
-      </c>
-      <c r="K117">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="118" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B118" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C118" t="s">
-        <v>142</v>
-      </c>
-      <c r="D118" t="s">
-        <v>143</v>
-      </c>
-      <c r="K118">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="119" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B119" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C119" t="s">
-        <v>144</v>
-      </c>
-      <c r="D119" t="s">
-        <v>144</v>
-      </c>
-      <c r="K119">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="120" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B120" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C120" t="s">
-        <v>145</v>
-      </c>
-      <c r="D120" t="s">
-        <v>145</v>
-      </c>
-      <c r="K120">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="121" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B121" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C121" t="s">
-        <v>146</v>
-      </c>
-      <c r="D121" t="s">
-        <v>146</v>
-      </c>
-      <c r="K121">
-        <v>69</v>
-      </c>
-      <c r="L121">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B122" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C122" t="s">
-        <v>147</v>
-      </c>
-      <c r="D122" t="s">
-        <v>147</v>
-      </c>
-      <c r="K122">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="123" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B123" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C123" t="s">
-        <v>148</v>
-      </c>
-      <c r="D123" t="s">
-        <v>148</v>
-      </c>
-      <c r="K123">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="124" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B124" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C124" t="s">
-        <v>149</v>
-      </c>
-      <c r="D124" t="s">
-        <v>149</v>
-      </c>
-      <c r="K124">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="125" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B125" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C125" t="s">
-        <v>150</v>
-      </c>
-      <c r="D125" t="s">
-        <v>150</v>
-      </c>
-      <c r="K125">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="126" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B126" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C126" t="s">
-        <v>151</v>
-      </c>
-      <c r="D126" t="s">
-        <v>152</v>
-      </c>
-      <c r="K126">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="127" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B127" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C127" t="s">
-        <v>153</v>
-      </c>
-      <c r="D127" t="s">
-        <v>153</v>
-      </c>
-      <c r="K127">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="128" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B128" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C128" t="s">
-        <v>154</v>
-      </c>
-      <c r="D128" t="s">
-        <v>154</v>
-      </c>
-      <c r="K128">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="129" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B129" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C129" t="s">
-        <v>155</v>
-      </c>
-      <c r="D129" t="s">
-        <v>155</v>
-      </c>
-      <c r="K129">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="130" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B130" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C130" t="s">
-        <v>156</v>
-      </c>
-      <c r="D130" t="s">
-        <v>156</v>
-      </c>
-      <c r="K130">
-        <v>78</v>
-      </c>
-      <c r="L130">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="131" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B131" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C131" t="s">
-        <v>157</v>
-      </c>
-      <c r="D131" t="s">
-        <v>157</v>
-      </c>
-      <c r="K131">
-        <v>79</v>
-      </c>
-      <c r="L131">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="132" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B132" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C132" t="s">
-        <v>158</v>
-      </c>
-      <c r="D132" t="s">
-        <v>158</v>
-      </c>
-      <c r="K132">
-        <v>80</v>
-      </c>
-      <c r="L132">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="133" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B133" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C133" t="s">
-        <v>159</v>
-      </c>
-      <c r="D133" t="s">
-        <v>159</v>
-      </c>
-      <c r="K133">
-        <v>81</v>
-      </c>
-      <c r="L133">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="134" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B134" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C134" t="s">
-        <v>104</v>
-      </c>
-      <c r="D134" t="s">
-        <v>105</v>
-      </c>
-      <c r="K134">
-        <v>82</v>
-      </c>
-      <c r="L134">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B135" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C135" t="s">
-        <v>107</v>
-      </c>
-      <c r="D135" t="s">
-        <v>108</v>
-      </c>
-      <c r="K135">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="136" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B136" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C136" t="s">
-        <v>109</v>
-      </c>
-      <c r="D136" t="s">
-        <v>110</v>
-      </c>
-      <c r="K136">
-        <v>84</v>
-      </c>
-      <c r="L136">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B137" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C137" t="s">
-        <v>112</v>
-      </c>
-      <c r="D137" t="s">
-        <v>113</v>
-      </c>
-      <c r="K137">
-        <v>85</v>
-      </c>
-      <c r="L137">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B138" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C138" t="s">
-        <v>178</v>
-      </c>
-      <c r="D138" t="s">
-        <v>178</v>
-      </c>
-      <c r="K138">
-        <v>86</v>
-      </c>
-      <c r="L138">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="139" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B139" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C139" t="s">
-        <v>114</v>
-      </c>
-      <c r="D139" t="s">
-        <v>508</v>
-      </c>
-      <c r="K139">
-        <v>87</v>
-      </c>
-      <c r="L139">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="140" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B140" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C140" t="s">
-        <v>116</v>
-      </c>
-      <c r="D140" t="s">
-        <v>509</v>
-      </c>
-      <c r="K140">
-        <v>88</v>
-      </c>
-      <c r="L140">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="141" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B141" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C141" t="s">
-        <v>118</v>
-      </c>
-      <c r="D141" t="s">
-        <v>510</v>
-      </c>
-      <c r="K141">
-        <v>89</v>
-      </c>
-      <c r="L141">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B142" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C142" t="s">
-        <v>120</v>
-      </c>
-      <c r="D142" t="s">
-        <v>511</v>
-      </c>
-      <c r="K142">
-        <v>90</v>
-      </c>
-      <c r="L142">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B143" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C143" t="s">
-        <v>122</v>
-      </c>
-      <c r="D143" t="s">
-        <v>123</v>
-      </c>
-      <c r="K143">
-        <v>91</v>
-      </c>
-      <c r="L143">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B144" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C144" t="s">
-        <v>164</v>
-      </c>
-      <c r="D144" t="s">
-        <v>165</v>
-      </c>
-      <c r="K144">
-        <v>92</v>
-      </c>
-      <c r="L144">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B145" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C145" t="s">
-        <v>125</v>
-      </c>
-      <c r="D145" t="s">
-        <v>126</v>
-      </c>
-      <c r="K145">
-        <v>93</v>
-      </c>
-      <c r="L145">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B146" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C146" t="s">
-        <v>166</v>
-      </c>
-      <c r="D146" t="s">
-        <v>167</v>
-      </c>
-      <c r="K146">
-        <v>94</v>
-      </c>
-      <c r="L146">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B147" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C147" t="s">
-        <v>127</v>
-      </c>
-      <c r="D147" t="s">
-        <v>128</v>
-      </c>
-      <c r="K147">
-        <v>95</v>
-      </c>
-      <c r="L147">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="148" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B148" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C148" t="s">
-        <v>168</v>
-      </c>
-      <c r="D148" t="s">
-        <v>169</v>
-      </c>
-      <c r="K148">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="149" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B149" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C149" t="s">
-        <v>129</v>
-      </c>
-      <c r="D149" t="s">
-        <v>130</v>
-      </c>
-      <c r="K149">
-        <v>97</v>
-      </c>
-      <c r="L149">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B150" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C150" t="s">
-        <v>170</v>
-      </c>
-      <c r="D150" t="s">
-        <v>171</v>
-      </c>
-      <c r="K150">
-        <v>98</v>
-      </c>
-      <c r="L150">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="151" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B151" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C151" t="s">
-        <v>131</v>
-      </c>
-      <c r="D151" t="s">
-        <v>131</v>
-      </c>
-      <c r="K151">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="152" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B152" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C152" t="s">
-        <v>134</v>
-      </c>
-      <c r="D152" t="s">
-        <v>135</v>
-      </c>
-      <c r="K152">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="153" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B153" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C153" t="s">
-        <v>136</v>
-      </c>
-      <c r="D153" t="s">
-        <v>137</v>
-      </c>
-      <c r="K153">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="154" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B154" s="112" t="s">
-        <v>506</v>
-      </c>
-      <c r="C154" t="s">
-        <v>204</v>
-      </c>
-      <c r="D154" t="s">
-        <v>204</v>
-      </c>
-      <c r="K154">
-        <v>102</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
Initial test run and updates to Modify Table tool: - Ran first test run of the tool - Updated condition for common error field name - Changed input layer parameter from layer name to layer path
</commit_message>
<xml_diff>
--- a/configuration/fields.xlsx
+++ b/configuration/fields.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tauex-my.sharepoint.com/personal/kerenha_tauex_tau_ac_il/Documents/Documents/ArcGIS/pty_framework/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="445" documentId="13_ncr:1_{42DDB87E-81E9-4226-9973-413C4AA9401D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04B49F21-9103-48AE-998F-E6100F907CD6}"/>
+  <xr:revisionPtr revIDLastSave="447" documentId="13_ncr:1_{42DDB87E-81E9-4226-9973-413C4AA9401D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47BCC607-ED7B-4E36-96D2-A183F8A0150F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="673" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="673" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3088" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3089" uniqueCount="514">
   <si>
     <t>OBJECTID</t>
   </si>
@@ -10017,8 +10017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B81B3B6-A5EA-43DC-9DF2-5745324BB6CB}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B24" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44:H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -10497,7 +10497,7 @@
         <v>451</v>
       </c>
       <c r="C21" s="103" t="s">
-        <v>452</v>
+        <v>430</v>
       </c>
       <c r="D21" s="104" t="s">
         <v>437</v>
@@ -11087,7 +11087,9 @@
       </c>
       <c r="F45" s="104"/>
       <c r="G45" s="105"/>
-      <c r="H45" s="104"/>
+      <c r="H45" s="100" t="s">
+        <v>505</v>
+      </c>
       <c r="I45">
         <v>1</v>
       </c>

</xml_diff>